<commit_message>
Update database design and generated Table scripts
</commit_message>
<xml_diff>
--- a/Documents/Design Document.xlsx
+++ b/Documents/Design Document.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="113">
   <si>
     <t>Database : SecureChat</t>
   </si>
@@ -132,24 +132,15 @@
     <t>Country</t>
   </si>
   <si>
-    <t>FK_USR_Country_TLM_ID</t>
-  </si>
-  <si>
     <t>PhoneNumber</t>
   </si>
   <si>
-    <t>VARCHAR (10)</t>
-  </si>
-  <si>
     <t>EmailID</t>
   </si>
   <si>
     <t>CreatedBy</t>
   </si>
   <si>
-    <t>TBL_LOOKUP_MST (ID)</t>
-  </si>
-  <si>
     <t>TBL_USER (ID)</t>
   </si>
   <si>
@@ -174,9 +165,6 @@
     <t>DATETIME</t>
   </si>
   <si>
-    <t>CURRENT_DATE</t>
-  </si>
-  <si>
     <t>ModifiedBy</t>
   </si>
   <si>
@@ -186,27 +174,15 @@
     <t>ModifiedOn</t>
   </si>
   <si>
-    <t>DF_CreatedON</t>
-  </si>
-  <si>
-    <t>DF_ModifiedOn</t>
-  </si>
-  <si>
     <t>IsActive</t>
   </si>
   <si>
     <t>BOOLEAN</t>
   </si>
   <si>
-    <t>DF_IsActive</t>
-  </si>
-  <si>
     <t>IsDeleted</t>
   </si>
   <si>
-    <t>DF_IsDeleted</t>
-  </si>
-  <si>
     <t>Unique</t>
   </si>
   <si>
@@ -225,9 +201,6 @@
     <t>Verify and Register</t>
   </si>
   <si>
-    <t>Is this field requred?</t>
-  </si>
-  <si>
     <t>Description: This table contains user information</t>
   </si>
   <si>
@@ -300,9 +273,6 @@
     <t>VARCHAR(10)</t>
   </si>
   <si>
-    <t>UK_CountryCode</t>
-  </si>
-  <si>
     <t>Descreption: This table contains the country related data.</t>
   </si>
   <si>
@@ -328,6 +298,69 @@
   </si>
   <si>
     <t>Send message</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>UsrPassword</t>
+  </si>
+  <si>
+    <t>TBL_COUNTRY_MST(ID)</t>
+  </si>
+  <si>
+    <t>FK_USR_Country_TCM_ID</t>
+  </si>
+  <si>
+    <t>FK_TCM_CreatedBy_USR_ID</t>
+  </si>
+  <si>
+    <t>FK_TCM_ModifiedBy_USR_ID</t>
+  </si>
+  <si>
+    <t>Table: TBL_LOG</t>
+  </si>
+  <si>
+    <t>TBL_LOG</t>
+  </si>
+  <si>
+    <t>LOG</t>
+  </si>
+  <si>
+    <t>Descreption: This table will maintain the logs of application.</t>
+  </si>
+  <si>
+    <t>ErrorCode</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>VARCHAR(500)</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>FunctionName</t>
+  </si>
+  <si>
+    <t>LogDateTime</t>
+  </si>
+  <si>
+    <t>FK_LOG_CreatedBy_USR_ID</t>
+  </si>
+  <si>
+    <t>FK_LOG_ModifiedBy_USR_ID</t>
+  </si>
+  <si>
+    <t>ModuleName</t>
   </si>
 </sst>
 </file>
@@ -351,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,12 +412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -553,15 +580,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -858,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,22 +902,22 @@
     <col min="10" max="10" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
@@ -911,7 +937,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>7</v>
@@ -923,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>1</v>
       </c>
@@ -947,7 +973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>2</v>
       </c>
@@ -968,16 +994,13 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
-      <c r="K7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>3</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>34</v>
@@ -994,7 +1017,7 @@
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>4</v>
       </c>
@@ -1012,27 +1035,27 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>5</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21" t="s">
@@ -1041,15 +1064,15 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>6</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>34</v>
@@ -1066,12 +1089,12 @@
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>7</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>11</v>
@@ -1084,42 +1107,40 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>9</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>11</v>
@@ -1132,45 +1153,43 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>10</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>11</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
@@ -1182,19 +1201,17 @@
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
-        <v>58</v>
-      </c>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>12</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="s">
@@ -1206,20 +1223,18 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
-      <c r="J17" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="J17" s="21"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1242,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H21" s="22" t="s">
         <v>7</v>
@@ -1303,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>11</v>
@@ -1323,10 +1338,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>32</v>
@@ -1341,7 +1356,7 @@
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1349,15 +1364,15 @@
         <v>5</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="21"/>
@@ -1371,13 +1386,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="21"/>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="21"/>
@@ -1391,7 +1406,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>11</v>
@@ -1404,10 +1419,10 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1415,31 +1430,29 @@
         <v>8</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="21" t="s">
-        <v>54</v>
-      </c>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>9</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>11</v>
@@ -1452,10 +1465,10 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1463,34 +1476,32 @@
         <v>10</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="21" t="s">
-        <v>55</v>
-      </c>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>11</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21" t="s">
@@ -1502,19 +1513,17 @@
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="21" t="s">
-        <v>58</v>
-      </c>
+      <c r="J32" s="21"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>12</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21" t="s">
@@ -1526,18 +1535,16 @@
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="J33" s="21"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1560,7 +1567,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H37" s="22" t="s">
         <v>7</v>
@@ -1600,60 +1607,56 @@
       <c r="A39" s="21">
         <v>2</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>86</v>
+      <c r="B39" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="I39" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="J39" s="24" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
         <v>3</v>
       </c>
-      <c r="B40" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>91</v>
+      <c r="B40" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="21"/>
-      <c r="G40" s="21" t="s">
-        <v>13</v>
-      </c>
+      <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
-      <c r="J40" s="24" t="s">
-        <v>92</v>
-      </c>
+      <c r="J40" s="23"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>4</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>11</v>
@@ -1666,10 +1669,10 @@
       <c r="G41" s="21"/>
       <c r="H41" s="21"/>
       <c r="I41" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1678,24 +1681,22 @@
         <v>5</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G42" s="21"/>
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="21" t="s">
-        <v>54</v>
-      </c>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
@@ -1703,7 +1704,7 @@
         <v>6</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>11</v>
@@ -1716,10 +1717,10 @@
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1728,24 +1729,22 @@
         <v>7</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="21" t="s">
-        <v>55</v>
-      </c>
+      <c r="J44" s="21"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="21">
@@ -1753,10 +1752,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21" t="s">
@@ -1768,9 +1767,7 @@
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="21" t="s">
-        <v>58</v>
-      </c>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="21">
@@ -1778,10 +1775,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="21" t="s">
@@ -1793,9 +1790,345 @@
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
+        <v>1</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="21">
+        <v>2</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="21">
+        <v>3</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="21">
+        <v>4</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="21">
+        <v>5</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="21">
+        <v>6</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="21">
+        <f>A56+1</f>
+        <v>7</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <f t="shared" ref="A58:A62" si="1">A57+1</f>
+        <v>8</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="21">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="21">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="21">
+        <v>1</v>
+      </c>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="21">
+        <v>13</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="21">
+        <v>0</v>
+      </c>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,7 +2140,7 @@
   <dimension ref="A2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,10 +2152,10 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1830,10 +2163,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1841,10 +2174,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1852,16 +2185,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="21">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
@@ -1943,7 +2282,7 @@
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,13 +2324,13 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="P6">
         <v>3</v>
       </c>
       <c r="Q6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2009,14 +2348,14 @@
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="28"/>
+      <c r="Q8" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="27"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -2029,7 +2368,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="6"/>
       <c r="J9" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -2037,14 +2376,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="6"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="31"/>
+      <c r="Q9" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="30"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
@@ -2111,12 +2450,12 @@
       <c r="N12" s="5"/>
       <c r="O12" s="6"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="37"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="36"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
@@ -2135,14 +2474,14 @@
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
       <c r="P13" s="5"/>
-      <c r="Q13" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="R13" s="39"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="37"/>
+      <c r="Q13" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="R13" s="38"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="36"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
@@ -2159,12 +2498,12 @@
       <c r="N14" s="5"/>
       <c r="O14" s="6"/>
       <c r="P14" s="5"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="37"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="36"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -2185,14 +2524,14 @@
       <c r="N15" s="5"/>
       <c r="O15" s="6"/>
       <c r="P15" s="5"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="V15" s="39"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="V15" s="38"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
@@ -2213,12 +2552,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="6"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="37"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="36"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
@@ -2235,12 +2574,12 @@
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="37"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="36"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -2259,12 +2598,12 @@
       <c r="N18" s="5"/>
       <c r="O18" s="6"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="37"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="36"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
@@ -2285,14 +2624,14 @@
       <c r="N19" s="5"/>
       <c r="O19" s="6"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="V19" s="39"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="V19" s="38"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
@@ -2371,27 +2710,27 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H23" s="19"/>
       <c r="J23" s="4"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="18" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="N23" s="18"/>
       <c r="O23" s="19"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="14" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
       <c r="V23" s="19" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
@@ -2409,12 +2748,12 @@
       <c r="N24" s="8"/>
       <c r="O24" s="9"/>
       <c r="P24" s="5"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="34"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>